<commit_message>
analisis de las 3 priemras simulaciones
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Simulaciones/proporciones/TEST_PROPORCIONES_240.xlsx
+++ b/codigo_final_organizado/Simulaciones/proporciones/TEST_PROPORCIONES_240.xlsx
@@ -540,7 +540,7 @@
         <v>0.5736916076074339</v>
       </c>
       <c r="P2">
-        <v>1.184599613078336</v>
+        <v>1.173940532471115</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -590,7 +590,7 @@
         <v>0.6603266932837247</v>
       </c>
       <c r="P3">
-        <v>0.6638869517475086</v>
+        <v>0.6687495246397893</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -640,7 +640,7 @@
         <v>0.5657780740147028</v>
       </c>
       <c r="P4">
-        <v>0.6553335718387399</v>
+        <v>0.6450408693787498</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -690,7 +690,7 @@
         <v>0.6704870156335671</v>
       </c>
       <c r="P5">
-        <v>0.6753547673184215</v>
+        <v>0.6581965283700736</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -740,7 +740,7 @@
         <v>0.6003642030260389</v>
       </c>
       <c r="P6">
-        <v>0.7871601135773946</v>
+        <v>0.7599649704893262</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -790,7 +790,7 @@
         <v>0.5875417680951129</v>
       </c>
       <c r="P7">
-        <v>1.564128717685957</v>
+        <v>1.526723262206673</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -840,7 +840,7 @@
         <v>0.6417321975538176</v>
       </c>
       <c r="P8">
-        <v>0.6672659829553463</v>
+        <v>0.6571205391460256</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -890,7 +890,7 @@
         <v>0.5775164906182478</v>
       </c>
       <c r="P9">
-        <v>0.6345558355020432</v>
+        <v>0.6334061194151843</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -940,7 +940,7 @@
         <v>0.7026119061977654</v>
       </c>
       <c r="P10">
-        <v>0.7186655671854139</v>
+        <v>0.7033441035257412</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -990,7 +990,7 @@
         <v>0.6084337161663037</v>
       </c>
       <c r="P11">
-        <v>0.7453186664408222</v>
+        <v>0.7651462897421865</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1040,7 +1040,7 @@
         <v>0.579367170653891</v>
       </c>
       <c r="P12">
-        <v>0.7838255243523483</v>
+        <v>0.7580490425937152</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1090,7 +1090,7 @@
         <v>0.7264253836893734</v>
       </c>
       <c r="P13">
-        <v>0.8855123732167788</v>
+        <v>0.8571530970826886</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1140,7 +1140,7 @@
         <v>0.6245230188783316</v>
       </c>
       <c r="P14">
-        <v>0.8304673070749259</v>
+        <v>0.8172362399217724</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1190,7 +1190,7 @@
         <v>0.5677156738271545</v>
       </c>
       <c r="P15">
-        <v>0.5847786898245868</v>
+        <v>0.5838850344709698</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1240,7 +1240,7 @@
         <v>0.5796479908554225</v>
       </c>
       <c r="P16">
-        <v>0.6339600222338873</v>
+        <v>0.6350345065702816</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1290,7 +1290,7 @@
         <v>0.573543970463101</v>
       </c>
       <c r="P17">
-        <v>0.5995499488858513</v>
+        <v>0.6002439556025914</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1340,7 +1340,7 @@
         <v>0.6242562037867097</v>
       </c>
       <c r="P18">
-        <v>0.574111738924885</v>
+        <v>0.5742170078473631</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1390,7 +1390,7 @@
         <v>0.5618756364068193</v>
       </c>
       <c r="P19">
-        <v>0.709693461714437</v>
+        <v>0.7177770347464668</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1440,7 +1440,7 @@
         <v>0.6336554373047861</v>
       </c>
       <c r="P20">
-        <v>1.187763835633186</v>
+        <v>1.205769495845655</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1490,7 +1490,7 @@
         <v>0.6968446118267755</v>
       </c>
       <c r="P21">
-        <v>0.5599956020556088</v>
+        <v>0.5594446828765947</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1540,7 +1540,7 @@
         <v>0.581901186022683</v>
       </c>
       <c r="P22">
-        <v>0.6039879091676288</v>
+        <v>0.6052881758016058</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1590,7 +1590,7 @@
         <v>0.5633282189183026</v>
       </c>
       <c r="P23">
-        <v>0.6601260883882234</v>
+        <v>0.6612256998766306</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1640,7 +1640,7 @@
         <v>0.5786979494519991</v>
       </c>
       <c r="P24">
-        <v>0.6202242330382429</v>
+        <v>0.6207933488881647</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1690,7 +1690,7 @@
         <v>0.5848924932765067</v>
       </c>
       <c r="P25">
-        <v>0.6706416955880444</v>
+        <v>0.6709494555951921</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1740,7 +1740,7 @@
         <v>0.6038308019921882</v>
       </c>
       <c r="P26">
-        <v>0.5947176417899049</v>
+        <v>0.5945000833547658</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1790,7 +1790,7 @@
         <v>0.5958491811777039</v>
       </c>
       <c r="P27">
-        <v>0.6666292389370406</v>
+        <v>0.6690940401230234</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -1840,7 +1840,7 @@
         <v>0.5927991125843107</v>
       </c>
       <c r="P28">
-        <v>1.40762763165843</v>
+        <v>1.386192599252586</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1890,7 +1890,7 @@
         <v>0.5686782175211413</v>
       </c>
       <c r="P29">
-        <v>3.197478273820519</v>
+        <v>3.209388084453111</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -1940,7 +1940,7 @@
         <v>0.6279788112384055</v>
       </c>
       <c r="P30">
-        <v>2.855857420047128</v>
+        <v>2.875728074034313</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -1990,7 +1990,7 @@
         <v>0.6110563320814657</v>
       </c>
       <c r="P31">
-        <v>2.519088750654653</v>
+        <v>2.536223211262842</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -2040,7 +2040,7 @@
         <v>0.5604817918785853</v>
       </c>
       <c r="P32">
-        <v>3.187793747503262</v>
+        <v>3.209680883537202</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2090,7 +2090,7 @@
         <v>0.5968566028664319</v>
       </c>
       <c r="P33">
-        <v>2.938885543292998</v>
+        <v>2.951980627688052</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2140,7 +2140,7 @@
         <v>0.5858334451365965</v>
       </c>
       <c r="P34">
-        <v>2.577133896059669</v>
+        <v>2.581096709220017</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -2190,7 +2190,7 @@
         <v>0.6646590178714629</v>
       </c>
       <c r="P35">
-        <v>1.957707966312496</v>
+        <v>1.944977867088071</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -2240,7 +2240,7 @@
         <v>0.7153385182591763</v>
       </c>
       <c r="P36">
-        <v>1.938417621085461</v>
+        <v>1.902997215914106</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -2290,7 +2290,7 @@
         <v>0.9393428498484447</v>
       </c>
       <c r="P37">
-        <v>0.974841219240562</v>
+        <v>0.9311757893288353</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -2340,7 +2340,7 @@
         <v>0.6815495698168342</v>
       </c>
       <c r="P38">
-        <v>0.7909249856312531</v>
+        <v>0.7639131017440088</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -2390,7 +2390,7 @@
         <v>0.5772641649094832</v>
       </c>
       <c r="P39">
-        <v>0.7806039933979162</v>
+        <v>0.7865765523628162</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -2440,7 +2440,7 @@
         <v>0.6434865361676948</v>
       </c>
       <c r="P40">
-        <v>2.093863420725362</v>
+        <v>2.08999422632383</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -2490,7 +2490,7 @@
         <v>0.5878035026969112</v>
       </c>
       <c r="P41">
-        <v>0.6515156621174684</v>
+        <v>0.6512220892168789</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -2540,7 +2540,7 @@
         <v>0.5833485212860549</v>
       </c>
       <c r="P42">
-        <v>0.7205009708242128</v>
+        <v>0.7214535434586795</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -2590,7 +2590,7 @@
         <v>0.5835833044903995</v>
       </c>
       <c r="P43">
-        <v>0.5756001356637316</v>
+        <v>0.5752907435528255</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -2640,7 +2640,7 @@
         <v>0.6404439997457815</v>
       </c>
       <c r="P44">
-        <v>1.0836887707379</v>
+        <v>1.088286471391299</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -2690,7 +2690,7 @@
         <v>0.569965272697995</v>
       </c>
       <c r="P45">
-        <v>0.5908155472649602</v>
+        <v>0.5912974701318487</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -2740,7 +2740,7 @@
         <v>0.5726076318264537</v>
       </c>
       <c r="P46">
-        <v>0.5833604490621527</v>
+        <v>0.5819542572851222</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -2790,7 +2790,7 @@
         <v>0.5781085589016417</v>
       </c>
       <c r="P47">
-        <v>0.6361465534893634</v>
+        <v>0.6378035955409712</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -2840,7 +2840,7 @@
         <v>0.5808839461959651</v>
       </c>
       <c r="P48">
-        <v>0.5767530944741185</v>
+        <v>0.5757688880479208</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -2890,7 +2890,7 @@
         <v>0.5956350088899973</v>
       </c>
       <c r="P49">
-        <v>0.590681417905102</v>
+        <v>0.591550316930182</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -2940,7 +2940,7 @@
         <v>0.6198773273762356</v>
       </c>
       <c r="P50">
-        <v>0.5680727583437137</v>
+        <v>0.5679457863888585</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -2990,7 +2990,7 @@
         <v>0.6250128870866493</v>
       </c>
       <c r="P51">
-        <v>0.9750750290380591</v>
+        <v>0.9753587577666069</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -3040,7 +3040,7 @@
         <v>0.5842998672689498</v>
       </c>
       <c r="P52">
-        <v>1.2245434623583</v>
+        <v>1.223267635565539</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -3090,7 +3090,7 @@
         <v>0.5934641523719195</v>
       </c>
       <c r="P53">
-        <v>0.7313961542732569</v>
+        <v>0.7317666296063944</v>
       </c>
     </row>
   </sheetData>

</xml_diff>